<commit_message>
writing new part of L5
</commit_message>
<xml_diff>
--- a/lab4/lab4prob2soln.xlsx
+++ b/lab4/lab4prob2soln.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="260" windowWidth="25520" windowHeight="15620" tabRatio="500" activeTab="1"/>
+    <workbookView minimized="1" xWindow="520" yWindow="5320" windowWidth="25480" windowHeight="10920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>TIME</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t xml:space="preserve">R-K error/Δt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">dt </t>
+  </si>
+  <si>
+    <t>euler error</t>
+  </si>
+  <si>
+    <t>midpoint</t>
+  </si>
+  <si>
+    <t>RK</t>
   </si>
 </sst>
 </file>
@@ -157,8 +169,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,7 +241,7 @@
     <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="57">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -246,6 +266,10 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -270,6 +294,10 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -646,15 +674,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M32"/>
+  <dimension ref="B2:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="3" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
@@ -1415,6 +1444,86 @@
         <v>6.2472657300590137E-2</v>
       </c>
     </row>
+    <row r="35" spans="2:9">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C36" s="5">
+        <v>1.12E-4</v>
+      </c>
+      <c r="F36" s="5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1.2199999999999999E-9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="6">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="C37" s="5">
+        <v>2.9300000000000001E-5</v>
+      </c>
+      <c r="D37">
+        <f>(C36-C37)/(B36-B37)</f>
+        <v>6.6160000000000004E-3</v>
+      </c>
+      <c r="F37" s="5">
+        <v>1.2200000000000001E-7</v>
+      </c>
+      <c r="G37">
+        <f>(F36-F37)/(B36-B37)</f>
+        <v>7.0239999999999992E-5</v>
+      </c>
+      <c r="H37" s="5">
+        <v>7.5600000000000003E-11</v>
+      </c>
+      <c r="I37">
+        <f>H37/(B36-B37)</f>
+        <v>6.0479999999999998E-9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="6">
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="C38" s="5">
+        <v>1.95E-5</v>
+      </c>
+      <c r="D38">
+        <f>(C37-C38)/(B37-B38)</f>
+        <v>1.5680000000000002E-3</v>
+      </c>
+      <c r="F38" s="5">
+        <v>4.06E-8</v>
+      </c>
+      <c r="G38">
+        <f>(F37-F38)/(B37-B38)</f>
+        <v>1.3023999999999999E-5</v>
+      </c>
+      <c r="H38" s="5">
+        <v>7.93E-14</v>
+      </c>
+      <c r="I38">
+        <f>H38/(B37-B38)</f>
+        <v>1.2687999999999999E-11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>